<commit_message>
Add booking info Datum split, update pipelines for Booking Info column, add PROJECT_LOGIC.md
- Enhanced booking info extraction to strip 'Datum:' suffix from text
- Added Booking Info column to Excel output in pipelines.py
- Added PROJECT_LOGIC.md documentation
- Updated run_parallel.py with new nordiskamuseet URL
</commit_message>
<xml_diff>
--- a/event_category/events.xlsx
+++ b/event_category/events.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Events" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,76 +422,81 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>event_name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>location</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>time</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>event_url</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>end_date_iso</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>target_group</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>target_group_normalized</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>date_iso</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Event Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Date ISO</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Date ISO</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Target Group</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Target Group Normalized</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Booking Info</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Event URL</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MiniBio</t>
+          <t>Missa aldrig det roliga</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bokningen öppnar onsdag 7 januari 2026 08:00</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>09:30-10:45</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -513,7 +506,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://biblioteket.stockholm.se/forskolor</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -521,86 +514,272 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>scheduled</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Preschool</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>preschool_groups</t>
-        </is>
-      </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>Prenumerera på vårt nyhetsbrev så får du koll på evenemang, biljettsläpp och nya utställningar.</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>https://www.nordiskamuseet.se/evenemang/</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sagoyoga</t>
+          <t>Jullov på Nordiska museet</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Stockholms stadsbibliotek</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>09:15-09:45</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>No description provided in the text.</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://biblioteket.stockholm.se/forskolor</t>
+          <t>10:00-17:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Nordiska museet på Djurgården</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>Barn &amp; Familj</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>children</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>scheduled</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>förskolegrupper</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Gör en resa i tiden på jullovet på Nordiska museet på Djurgården! Vi har öppet alla dagar.</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>https://www.nordiskamuseet.se/evenemang/</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Pianomusik på nyårsafton</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-12-25</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-12-25</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>11:00-13:00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>STORA HALLEN</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>all_ages</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>2026-01-19</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>2026-01-19</t>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Ingår i ord. entré</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>https://www.nordiskamuseet.se/evenemang/</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Jullov på Nordiska museet</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2026-01-01</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2026-01-01</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2026-01-04</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>10:00-17:00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Nordiska museet på Djurgården</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Barn &amp; Familj</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>children</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Gör en resa i tiden på jullovet på Nordiska museet på Djurgården! Vi har öppet alla dagar.</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>https://www.nordiskamuseet.se/evenemang/</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Introduktion till Nordbor</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2026-01-01</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2026-01-01</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>STORA HALLEN</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>INGÅR I ORD. ENTRÉ</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>https://www.nordiskamuseet.se/evenemang/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement event date expansion and calendar date picker
- Add _expand_event_across_days() method to expand multi-day events into single-day entries
- Update get_events_filtered() to support filter_date parameter for date-specific filtering
- Add calendar date picker in filters to view events for a specific date
- Remove end_date display from event cards (events now show single dates after expansion)
- Add 'Filter By Date' selector with 'Date Range' and 'Specific Date' modes
- Events spanning multiple days now appear as separate entries for each day
- Users can now click a date on the calendar to see all events happening that day
</commit_message>
<xml_diff>
--- a/event_category/events.xlsx
+++ b/event_category/events.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +483,1556 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Christmas at Skansen</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2026-01-06</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>10:00-16:00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Concerts and performances</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Plan your visit by exploring the different activities along with details on dates, locations and, if not applicable during the whole day, hours.</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/christmas-at-skansen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Food and beverages at Bollnästorget</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>10:00-16:00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Bollnästorget</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Food and drinks</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>At Bollnästorget you can enjoy a varied selection of food and drinks in an inviting outdoor environment.</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>https://skansen.se/en/see-and-do/food-and-beverages/food-and-beverages-at-bollnastorget/</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Christmas in houses and farmsteads</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2026-01-06</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>10:00-15:00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>houses and farmsteads</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Cultural history</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Take a tour of Christmas celebrations from the 1830's and onwards. The bonfires are lit and the Christmas dinner tables from different time in history.</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/christmas-in-houses-and-farmsteads/</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Engineering workshop</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2026-01-06</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>10:00-16:00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Cultural history</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>The Engineering works (Mekaniska verkstaden) is based on a factory that was founded in 1889 and produced compression-ignition engines among its wares.</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/engineering-workshop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Delsbo Farmstead</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2026-01-06</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>10:00-16:00</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Delsbo Farmstead</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Cultural history</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>The Delsbo farmstead has magnificent wall paintings and rooms for entertaining and guests.</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/delsbo-farmstead/</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ironmonger’s apartment</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>10:00-16:00</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Cultural history</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>This apartment is occupied by the ironmonger and his family. They moved in and furnished their home in the early 1930s.</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/ironmongers-apartment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Seglora church</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2026-01-05</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>10:00-16:00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Seglora church</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Cultural history</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Seglora Church (Seglora kyrka) comes from a parish in Västergötland. The old wooden church dating from 1730 was abandoned when a new church, built of stone, was erected in 1903.</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/seglora-church/</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Farm Labourer’s cottage</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>10:00-16:00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Cultural history</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>The Farm Labourer’s Cottage (Statarlängan) contains dwellings for two families and shows how they lived about 1920.</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/farm-labourers-cottage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Hardware store</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2026-01-06</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>10:00-16:00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Cultural history</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>The period illustrated by the premises in the ironmongery, or hardware store, is the 1930s. The fittings date originally from the 1880s though the interior was partially modernized in the 1930s.</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/hardware-store/</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Skansen Museum Shop in the Lodge</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>10:00-16:00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>the Lodge</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Shops</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>In the Lodge by the Bollnäs square you find one of Skansen's museum shops. It's open in the summer and on holidays like the Advent weekends and on Chrismas Eve.</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/skansen-museum-shop-in-the-lodge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Lill-Skansen Museum Shop</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2026-01-04</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>10:00-15:00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Shops</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>In this shop you can find toys, games and animal toys along with books and other keepsakes.</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/lill-skansen-museum-shop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>New Year’s Eve</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2026-01-01</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2026-01-01</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>10.00-16.00, 20.00-24.00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Concerts and performances</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Welcome the new year with a stunning view over Stockholm as your back drop. Our New Year's celebration dates back to 1894 and is experienced at Solliden and via live broadcast on Swedish television.</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/new-years-eve/</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>New Year’s concert in Seglora Church</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2026-01-01</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2026-01-01</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>21.00, 22.00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Seglora Church</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Concerts and performances</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Welcome to Seglora Church on New Year's Eve to celebrate the start of the new year with beautiful music!</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>https://skansen.se/en/see-and-do/on-stage-activities/new-years-concert/</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Folk music in the Älvros Farmstead</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2026-01-02</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2026-01-02</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2026-01-06</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>12:00-14:30</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>the Älvros Farmstead</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Concerts and performances</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Folk music has a long tradition in Sweden and at Skansen. Come visit the Älvros Farmstead to hear Skansen's Folk Musicians play!</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/folk-music-in-the-alvros-farmstead/</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>The Bakery</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2026-01-03</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2026-01-03</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2026-01-04</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>10:00-16:00</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Food and drinks</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>The Bakery shows a bakery from the 1870s. Cinnamon Buns, bread and cookies can be bought at the counter alongside with coffee and tea.</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/the-bakery/</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Älvros Farmstead</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>10:00-15:00</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Älvros Farmstead</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Cultural history</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>The Älvros Farmstead shows what life was like at a farmstead in Härjedalen in northern Sweden. Here, the main way of life involved cattle breeding.</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/alvros-farmstead/</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Stockholm Glass Studio</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>10:00-16:00</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Shops</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>This is a glass studio from the 1930’s. Visitors can watch the skilled glassblower with traditional tools give life, form, light and colour to the glowing glass mass – a sight that has attracted people for generations.</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/stockholm-glass-studio/</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Old shop</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>10:00-15:00</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Cultural history</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>The Old Shop (Kryddboden) on the left as you enter displays a black brush, originally a gun brush, which was the traditional sign of grocers.</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/old-shop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Fishtalk – learn more about the Baltic Sea</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>11.00, 14.30</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>For children</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>children</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Learn more about the inhabitants in the Baltic sea</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/see-the-big-fishes-get-fed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Talk about horses (in Swedish)</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>For children</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>children</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Visit the stable and learn something new about our horses.</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/talk-about-horses-in-swedish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Meet a zookeeper at the Children’s zoo (in Swedish)</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>13:15</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>For children</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>children</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Skansen's zookeepers talk about the animal of the day at the Children's zoo.</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/todays-animal-at-the-childrens-zoo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Talk about the grey seal</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>For children</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>children</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Skansen's zookeepers feeds and talk about the grey seal at the upper seal enclosure. In Swedish.</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/talk-about-the-grey-seal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Snus and Match Museum</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>11:00-15:00</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Cultural history</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Snus and Match museum shows tobacco production in Sweden in the early 20th century and the development of the safety matches.</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/snus-and-match-museum/</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>The Printer’s Home</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>10:00-16:00</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Cultural history</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>The printer´s family lived in three rooms at the back of the printing office - a kitchen, drawing room and living room. The family ate and conducted their daily activities in the drawing room - where they also worked making the newspaper What´s New?.</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>https://skansen.se/en/the-printers-home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Väla school</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>10:00-16:00</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Skansen</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Cultural history</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>​Väla School (Väla skola) is an example of the vast number of schools that were built in the Swedish countryside in the middle of the 19th century.</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>https://www.skansen.se/en/see-and-do/non-bookable-activities/vala-school/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix National Museum event scraping and recurring events handling
- Updated universal_spider.py for better recurring event extraction
- Enhanced auto_selector_discovery.py for improved selector detection
- Updated db_manager.py for database handling improvements
- Added pagination_handler.py for dynamic content loading
- Added manual_selector_manager.py for manual selector management
- Added documentation for manual selector workflow and admin guide
- Updated admin_console.py with UI improvements
</commit_message>
<xml_diff>
--- a/event_category/events.xlsx
+++ b/event_category/events.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,17 +486,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Visning av samlingarna på svenska</t>
+          <t>Guidad visning: Hanna Hirsch Pauli</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>30 DECEMBER 14:00 - 15:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -531,29 +531,29 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Följ med på en visning där vi tittar närmare på konsten i museets samlingar. Från 1500-tal till nutid.</t>
+          <t>Gå med på en visning och upptäck konstnären bakom den älskade målningen Frukostdags. Hanna Hirsch Pauli kunde konsten att med sin lätta pensel förmedla känslan av en sommardag i det gröna eller den intima samvaron under en fotogenlampa. Tillsammans med en av museets pedagoger får du lära känna personen bakom konstverken: en karismatisk, frihetssökande kvinna mitt i centrum av förra sekelskiftets kulturliv.</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>https://www.nationalmuseum.se/kalendarium</t>
+          <t>https://www.nationalmuseum.se/guidad-visning-hanna-hirsch-pauli</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Öppen ateljé – drop-in för alla åldrar</t>
+          <t>Jullov i ateljéerna</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -563,7 +563,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>2 JANUARI 13:00 - 16:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -588,29 +588,29 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Välkommen till Ateljéerna! Här kan du måla, skulptera och skapa fritt med inspiration från konsten i museet.</t>
+          <t>Vill du prova på att skapa bilder på ett magiskt och enkelt sätt? Kom till jullovsateljén och testa monotypi, en spännande tryckteknik där du rollar på färg, ritar och spårar i den. Sedan ett snabbt svisch! På med papper och tryck till. Ingen bild blir den andra lik! Fri entré. Drop-in i mån av plats.</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>https://www.nationalmuseum.se/kalendarium</t>
+          <t>https://www.nationalmuseum.se/jullov</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Visning av samlingarna på svenska</t>
+          <t>Guidad visning: Hanna Hirsch Pauli</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -620,7 +620,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>2 JANUARI 14:00 - 15:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -645,29 +645,29 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Följ med på en visning där vi tittar närmare på konsten i museets samlingar. Från 1500-tal till nutid.</t>
+          <t>Gå med på en visning och upptäck konstnären bakom den älskade målningen Frukostdags. Hanna Hirsch Pauli kunde konsten att med sin lätta pensel förmedla känslan av en sommardag i det gröna eller den intima samvaron under en fotogenlampa. Tillsammans med en av museets pedagoger får du lära känna personen bakom konstverken: en karismatisk, frihetssökande kvinna mitt i centrum av förra sekelskiftets kulturliv.</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>https://www.nationalmuseum.se/kalendarium</t>
+          <t>https://www.nationalmuseum.se/guidad-visning-hanna-hirsch-pauli</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Öppen ateljé – drop-in för alla åldrar</t>
+          <t>Jullov i ateljéerna</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -677,7 +677,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>3 JANUARI 13:00 - 16:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -702,29 +702,29 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Välkommen till Ateljéerna! Här kan du måla, skulptera och skapa fritt med inspiration från konsten i museet.</t>
+          <t>Vill du prova på att skapa bilder på ett magiskt och enkelt sätt? Kom till jullovsateljén och testa monotypi, en spännande tryckteknik där du rollar på färg, ritar och spårar i den. Sedan ett snabbt svisch! På med papper och tryck till. Ingen bild blir den andra lik! Fri entré. Drop-in i mån av plats.</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>https://www.nationalmuseum.se/kalendarium</t>
+          <t>https://www.nationalmuseum.se/jullov</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Visning av samlingarna på svenska</t>
+          <t>Guidad visning: Samlingarna</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -734,7 +734,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>3 JANUARI 14:00 - 15:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -759,29 +759,29 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Följ med på en visning där vi tittar närmare på konsten i museets samlingar. Från 1500-tal till nutid.</t>
+          <t>Följ med på en guidad visning genom museet där pedagogen blandar berättelser om museets historia med fördjupningar om några av samlingarnas fantastiska konstverk.</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>https://www.nationalmuseum.se/kalendarium</t>
+          <t>https://www.nationalmuseum.se/guidad-visning-samlingarna</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Öppen ateljé – drop-in för alla åldrar</t>
+          <t>Guidad visning: Hanna Hirsch Pauli</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>3 JANUARI 15:30 - 16:30</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -816,29 +816,29 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Välkommen till Ateljéerna! Här kan du måla, skulptera och skapa fritt med inspiration från konsten i museet.</t>
+          <t>Gå med på en visning och upptäck konstnären bakom den älskade målningen Frukostdags. Hanna Hirsch Pauli kunde konsten att med sin lätta pensel förmedla känslan av en sommardag i det gröna eller den intima samvaron under en fotogenlampa. Tillsammans med en av museets pedagoger får du lära känna personen bakom konstverken: en karismatisk, frihetssökande kvinna mitt i centrum av förra sekelskiftets kulturliv.</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>https://www.nationalmuseum.se/kalendarium</t>
+          <t>https://www.nationalmuseum.se/guidad-visning-hanna-hirsch-pauli</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Visning av samlingarna på svenska</t>
+          <t>Jullov i ateljéerna</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>4 JANUARI 13:00 - 16:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -873,29 +873,29 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Följ med på en visning där vi tittar närmare på konsten i museets samlingar. Från 1500-tal till nutid.</t>
+          <t>Vill du prova på att skapa bilder på ett magiskt och enkelt sätt? Kom till jullovsateljén och testa monotypi, en spännande tryckteknik där du rollar på färg, ritar och spårar i den. Sedan ett snabbt svisch! På med papper och tryck till. Ingen bild blir den andra lik! Fri entré. Drop-in i mån av plats.</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>https://www.nationalmuseum.se/kalendarium</t>
+          <t>https://www.nationalmuseum.se/jullov</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Öppen ateljé – drop-in för alla åldrar</t>
+          <t>Guidad visning: Porträtt!</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -905,7 +905,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>4 JANUARI 14:00 - 15:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -930,29 +930,29 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Välkommen till Ateljéerna! Här kan du måla, skulptera och skapa fritt med inspiration från konsten i museet.</t>
+          <t>Gå med på en visning av utställningen Porträtt! – en resa från 1500-talet till idag fylld av avbildade människor. Du möter kungligheter, konstnärer, näringslivsprofiler och andra som på olika sätt valts ut och porträtterats i sin tid.</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>https://www.nationalmuseum.se/kalendarium</t>
+          <t>https://www.nationalmuseum.se/guidad-visning-porträtt</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Visning av samlingarna på svenska</t>
+          <t>Guidad visning: Hanna Hirsch Pauli</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -962,7 +962,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>4 JANUARI 15:30 - 16:30</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -987,69 +987,2431 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Följ med på en visning där vi tittar närmare på konsten i museets samlingar. Från 1500-tal till nutid.</t>
+          <t>Gå med på en visning och upptäck konstnären bakom den älskade målningen Frukostdags. Hanna Hirsch Pauli kunde konsten att med sin lätta pensel förmedla känslan av en sommardag i det gröna eller den intima samvaron under en fotogenlampa. Tillsammans med en av museets pedagoger får du lära känna personen bakom konstverken: en karismatisk, frihetssökande kvinna mitt i centrum av förra sekelskiftets kulturliv.</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>https://www.nationalmuseum.se/kalendarium</t>
+          <t>https://www.nationalmuseum.se/guidad-visning-hanna-hirsch-pauli</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Öppen ateljé – drop-in för alla åldrar</t>
+          <t>Guidad visning: Samlingarna</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>7 JANUARI 11:30 - 12:30</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Följ med på en guidad visning genom museet där pedagogen blandar berättelser om museets historia med fördjupningar om några av samlingarnas fantastiska konstverk.</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-samlingarna</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Guidad visning: Porträtt!</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>8 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Gå med på en visning av utställningen Porträtt! – en resa från 1500-talet till idag fylld av avbildade människor. Du möter kungligheter, konstnärer, näringslivsprofiler och andra som på olika sätt valts ut och porträtterats i sin tid.</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-porträtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Guidad visning: Samlingarna</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>10 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Följ med på en guidad visning genom museet där pedagogen blandar berättelser om museets historia med fördjupningar om några av samlingarnas fantastiska konstverk.</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-samlingarna</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Guidad visning: Porträtt!</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>2026-01-11</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>2026-01-11</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>all_ages</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>scheduled</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Välkommen till Ateljéerna! Här kan du måla, skulptera och skapa fritt med inspiration från konsten i museet.</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>https://www.nationalmuseum.se/kalendarium</t>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>11 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Gå med på en visning av utställningen Porträtt! – en resa från 1500-talet till idag fylld av avbildade människor. Du möter kungligheter, konstnärer, näringslivsprofiler och andra som på olika sätt valts ut och porträtterats i sin tid.</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-porträtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Introduktion till Nationalmuseum</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>13 JANUARI 13:00 - 13:20</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Välkommen till Nationalmuseum – Sveriges konst- och designmuseum! Med den här korta introduktionen bjuder vi in dig till att upptäcka ett urval höjdpunkter i museets samlingar som spänner över mer än sexhundra år. En av museets guider berättar och visar bilder. Gratis.</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/introduktion-till-nationalmuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Guidad visning: Porträtt!</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>13 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Gå med på en visning av utställningen Porträtt! – en resa från 1500-talet till idag fylld av avbildade människor. Du möter kungligheter, konstnärer, näringslivsprofiler och andra som på olika sätt valts ut och porträtterats i sin tid.</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-porträtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Introduktion till Nationalmuseum</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>14 JANUARI 13:00 - 13:20</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Välkommen till Nationalmuseum – Sveriges konst- och designmuseum! Med den här korta introduktionen bjuder vi in dig till att upptäcka ett urval höjdpunkter i museets samlingar som spänner över mer än sexhundra år. En av museets guider berättar och visar bilder. Gratis.</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/introduktion-till-nationalmuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Guidad visning: Nationalmuseum på 60 minuter</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>14 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>I den här guidade visningen ger vi oss ut på en upptäcktsfärd bland samlingarna och gör några utvalda nedslag inom konst, konsthantverk och design. Upplev både nyförvärvade konstverk och äldre favoriter.</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-nationalmuseum-på-60-minuter</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Guidad visning: Porträtt!</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2026-01-15</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2026-01-15</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>15 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Gå med på en visning av utställningen Porträtt! – en resa från 1500-talet till idag fylld av avbildade människor. Du möter kungligheter, konstnärer, näringslivsprofiler och andra som på olika sätt valts ut och porträtterats i sin tid.</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-porträtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Babyvisning: Siden, rysch och pysch</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2026-01-16</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2026-01-16</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>16 JANUARI 13:00 - 14:30</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Babies</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>babies</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Babyvisning på Nationalmuseum för nyfikna vuxna med barn i sitt- och krypålder (3–11 mån). Vi tittar på 1700-talsporträtt, och chillar med bebisarna. I ateljén blir det tyllhav à la Rokoko.</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/babyvisning-siden-rysch-och-pysch</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>NM Skulpturkroki</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2026-01-17</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2026-01-17</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>17 JANUARI 11:00 - 14:00</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Prova på att teckna kroki med skulpturer som modeller. Vi tecknar dem ur olika vinklar och i olika tempo och övar ögat i att se former, riktningar och rörelser i något som är helt stilla. Vässa blicken och njut av atmosfären i Skulpturgården – museets kanske vackraste rum!</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/skulpturkroki</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Guidad visning: Nationalmuseum på 60 minuter</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2026-01-17</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2026-01-17</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>17 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>I den här guidade visningen ger vi oss ut på en upptäcktsfärd bland samlingarna och gör några utvalda nedslag inom konst, konsthantverk och design. Upplev både nyförvärvade konstverk och äldre favoriter.</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-nationalmuseum-på-60-minuter</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Familjevisning: Nyfiken på färg!</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2026-01-17</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2026-01-17</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>17 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Families</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>families</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Följ med på en spännande och lekfull familjevisning där vi tillsammans upptäcker färgernas fantastiska värld i konsten</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/familjevisning-nyfiken-på-färg</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Guidad visning: Porträtt!</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2026-01-17</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2026-01-17</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>17 JANUARI 15:30 - 16:30</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Gå med på en visning av utställningen Porträtt! – en resa från 1500-talet till idag fylld av avbildade människor. Du möter kungligheter, konstnärer, näringslivsprofiler och andra som på olika sätt valts ut och porträtterats i sin tid.</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-porträtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>På engelska: Introduktion till Nationalmuseum</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>18 JANUARI 12:30 - 12:50</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Välkommen till Nationalmuseum – Sveriges konst- och designmuseum! Med den här korta introduktionen bjuder vi in dig till att upptäcka ett urval höjdpunkter i museets samlingar som spänner över mer än sexhundra år. En av museets kunniga guider berättar och visar bilder. På engelska.</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/på-engelska-introduktion-till-nationalmuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Introduktion till Nationalmuseum</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>18 JANUARI 13:00 - 13:20</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Välkommen till Nationalmuseum – Sveriges konst- och designmuseum! Med den här korta introduktionen bjuder vi in dig till att upptäcka ett urval höjdpunkter i museets samlingar som spänner över mer än sexhundra år. En av museets guider berättar och visar bilder. Gratis.</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/introduktion-till-nationalmuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Familjedag i ateljéerna</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>18 JANUARI 13:00 - 16:00</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Families</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>families</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>På söndagar utforskar vi olika material och tekniker i Nationalmuseums ateljéer. För barn från 4 år och vuxna tillsammans. Drop-in i mån av plats.</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/besök-museet/barn-och-familj/familjedag-i-ateljéerna</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Guidad visning: Porträtt!</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>18 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Gå med på en visning av utställningen Porträtt! – en resa från 1500-talet till idag fylld av avbildade människor. Du möter kungligheter, konstnärer, näringslivsprofiler och andra som på olika sätt valts ut och porträtterats i sin tid.</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-porträtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Introduktion till Nationalmuseum</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>20 JANUARI 13:00 - 13:20</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Välkommen till Nationalmuseum – Sveriges konst- och designmuseum! Med den här korta introduktionen bjuder vi in dig till att upptäcka ett urval höjdpunkter i museets samlingar som spänner över mer än sexhundra år. En av museets guider berättar och visar bilder. Gratis.</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/introduktion-till-nationalmuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Guidad visning: Porträtt!</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>20 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Gå med på en visning av utställningen Porträtt! – en resa från 1500-talet till idag fylld av avbildade människor. Du möter kungligheter, konstnärer, näringslivsprofiler och andra som på olika sätt valts ut och porträtterats i sin tid.</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-porträtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Introduktion till Nationalmuseum</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>21 JANUARI 13:00 - 13:20</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Välkommen till Nationalmuseum – Sveriges konst- och designmuseum! Med den här korta introduktionen bjuder vi in dig till att upptäcka ett urval höjdpunkter i museets samlingar som spänner över mer än sexhundra år. En av museets guider berättar och visar bilder. Gratis.</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/introduktion-till-nationalmuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Guidad visning: Nationalmuseum på 60 minuter</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>21 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>I den här guidade visningen ger vi oss ut på en upptäcktsfärd bland samlingarna och gör några utvalda nedslag inom konst, konsthantverk och design. Upplev både nyförvärvade konstverk och äldre favoriter.</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-nationalmuseum-på-60-minuter</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Guidad visning: Porträtt!</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>22 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Gå med på en visning av utställningen Porträtt! – en resa från 1500-talet till idag fylld av avbildade människor. Du möter kungligheter, konstnärer, näringslivsprofiler och andra som på olika sätt valts ut och porträtterats i sin tid.</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-porträtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Gratis kvällsdrop-in i ateljén</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>22 JANUARI 17:00 - 19:30</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Kom och var kreativ i Nationalmuseums ateljé! På torsdagskvällar kan du bekanta dig med några av konstens grundmaterial och tekniker. Prova på att teckna eller att måla med akvarell. Gratis drop-in. Inga förkunskaper behövs. Öppet för alla!</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/gratis-kvällsdrop-in-i-ateljén</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>NM Studio: Porträtt i kollageform med Emma Dominguez</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>22 JANUARI 17:30 - 20:00</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Är du mellan 17 och 29 år och sugen på att prova på olika konstnärliga material och tekniker? Kom till Nationalmuseums ateljé och NM Studio. I vårterminens första workshop får du öva på att berätta din egen historia och skapa ett eget porträtt genom collage tillsammans med konstnären Emma Dominguez.</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/nm-studio-porträtt-i-collageform-med-emma-dominguez</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Se mer i familjeporträtt från olika tider! Kom och samtala om konst</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>22 JANUARI 18:00 - 19:30</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Families</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>families</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Vill du se, prata om och utforska konst tillsammans med andra? I årets första tillfälle av samtalsserien Se Mer! pratar vi tillsammans om familjeporträtt – om bilder av nära, kära och arvfiender. Kom som du är inga förkunskaper eller förberedelser behövs.</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/se-mer-i-familjeporträtt-från-olika-tider-kom-och-samtala-om-konst</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Lördagsvisning: Att visa sig. Porträttet som makt och symbol</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2026-01-24</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2026-01-24</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>24 JANUARI 13:00 - 14:30</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Vem får synas – och hur? I en serie om tre fördjupande lördagsvisningar dyker vi ner i porträttets värld och utforskar allt från kunglig glans till dagens selfie-kultur. Den här gången tittar vi närmare på porträttet som makt och symbol.</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/lördagsvisning-att-visa-sig-porträttet-som-makt-och-symbol</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Guidad visning: Nationalmuseum på 60 minuter</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2026-01-24</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2026-01-24</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>24 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>I den här guidade visningen ger vi oss ut på en upptäcktsfärd bland samlingarna och gör några utvalda nedslag inom konst, konsthantverk och design. Upplev både nyförvärvade konstverk och äldre favoriter.</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-nationalmuseum-på-60-minuter</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Guidad visning: Porträtt!</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2026-01-24</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2026-01-24</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>24 JANUARI 15:30 - 16:30</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Gå med på en visning av utställningen Porträtt! – en resa från 1500-talet till idag fylld av avbildade människor. Du möter kungligheter, konstnärer, näringslivsprofiler och andra som på olika sätt valts ut och porträtterats i sin tid.</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-porträtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>På engelska: Introduktion till Nationalmuseum</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>25 JANUARI 12:30 - 12:50</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Välkommen till Nationalmuseum – Sveriges konst- och designmuseum! Med den här korta introduktionen bjuder vi in dig till att upptäcka ett urval höjdpunkter i museets samlingar som spänner över mer än sexhundra år. En av museets kunniga guider berättar och visar bilder. På engelska.</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/på-engelska-introduktion-till-nationalmuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Introduktion till Nationalmuseum</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>25 JANUARI 13:00 - 13:20</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Välkommen till Nationalmuseum – Sveriges konst- och designmuseum! Med den här korta introduktionen bjuder vi in dig till att upptäcka ett urval höjdpunkter i museets samlingar som spänner över mer än sexhundra år. En av museets guider berättar och visar bilder. Gratis.</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/introduktion-till-nationalmuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Familjedag i ateljéerna</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>25 JANUARI 13:00 - 16:00</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Families</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>families</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>På söndagar utforskar vi olika material och tekniker i Nationalmuseums ateljéer. För barn från 4 år och vuxna tillsammans. Drop-in i mån av plats.</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/besök-museet/barn-och-familj/familjedag-i-ateljéerna</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Guidad visning: Porträtt!</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>25 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Gå med på en visning av utställningen Porträtt! – en resa från 1500-talet till idag fylld av avbildade människor. Du möter kungligheter, konstnärer, näringslivsprofiler och andra som på olika sätt valts ut och porträtterats i sin tid.</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-porträtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Introduktion till Nationalmuseum</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>27 JANUARI 13:00 - 13:20</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Välkommen till Nationalmuseum – Sveriges konst- och designmuseum! Med den här korta introduktionen bjuder vi in dig till att upptäcka ett urval höjdpunkter i museets samlingar som spänner över mer än sexhundra år. En av museets guider berättar och visar bilder. Gratis.</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/introduktion-till-nationalmuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Guidad visning: Porträtt!</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>27 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>Gå med på en visning av utställningen Porträtt! – en resa från 1500-talet till idag fylld av avbildade människor. Du möter kungligheter, konstnärer, näringslivsprofiler och andra som på olika sätt valts ut och porträtterats i sin tid.</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-porträtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Introduktion till Nationalmuseum</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>28 JANUARI 13:00 - 13:20</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Välkommen till Nationalmuseum – Sveriges konst- och designmuseum! Med den här korta introduktionen bjuder vi in dig till att upptäcka ett urval höjdpunkter i museets samlingar som spänner över mer än sexhundra år. En av museets guider berättar och visar bilder. Gratis.</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/introduktion-till-nationalmuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Guidad visning: Nationalmuseum på 60 minuter</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>28 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>I den här guidade visningen ger vi oss ut på en upptäcktsfärd bland samlingarna och gör några utvalda nedslag inom konst, konsthantverk och design. Upplev både nyförvärvade konstverk och äldre favoriter.</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-nationalmuseum-på-60-minuter</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Guidad visning: Porträtt!</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>29 JANUARI 14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Gå med på en visning av utställningen Porträtt! – en resa från 1500-talet till idag fylld av avbildade människor. Du möter kungligheter, konstnärer, näringslivsprofiler och andra som på olika sätt valts ut och porträtterats i sin tid.</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/guidad-visning-porträtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Gratis kvällsdrop-in i ateljén</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>29 JANUARI 17:00 - 19:30</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Kom och var kreativ i Nationalmuseums ateljé! På torsdagskvällar kan du bekanta dig med några av konstens grundmaterial och tekniker. Prova på att teckna eller att måla med akvarell. Gratis drop-in. Inga förkunskaper behövs. Öppet för alla!</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/gratis-kvällsdrop-in-i-ateljén</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Torsdagskväll: Library Session med Sonic Erection</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>29 JANUARI 17:30 - 18:15</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Fri entré på Nationalmuseum på torsdagskvällar med konst, bar och musik. Det Stockholmsbaserade kollektivet Sonic Erection tillsammans med fanzinet Lucky4ever bjuder in till en stämningsfylld kväll i gamla biblioteket där text och poesi tillsammans med ambient musik skapar en audiovisuell helkroppsupplevelse. För dig mellan 17 och 29.</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/torsdagskväll-library-session-med-sonic-erection</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Konsten att dansa – prova på att dansa Bachata</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>29 JANUARI 17:30 - 19:30</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Välkommen till en ny programserie på torsdagskvällar med musik, rytm och dansglädje! Lär dig grunderna i Bachata och ge dig sen ut i dansens virvlar. Kom som du är, ensam eller med sällskap, öva, skratta, dansa och njut!</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/konsten-att-dansa</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Torsdagskväll: Library Session med Sonic Erection</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>29 JANUARI 19:00 - 19:45</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>all_ages</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>scheduled</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>Fri entré på Nationalmuseum på torsdagskvällar med konst, bar och musik. Det Stockholmsbaserade kollektivet Sonic Erection tillsammans med fanzinet Lucky4ever bjuder in till en stämningsfylld kväll i gamla biblioteket där text och poesi tillsammans med ambient musik skapar en audiovisuell helkroppsupplevelse. För dig mellan 17 och 29.</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>https://www.nationalmuseum.se/torsdagskväll-library-session-med-sonic-erection</t>
         </is>
       </c>
     </row>

</xml_diff>